<commit_message>
Script carga de productos actualizado
</commit_message>
<xml_diff>
--- a/import_data/product/inventario.xlsx
+++ b/import_data/product/inventario.xlsx
@@ -5107,20 +5107,20 @@
   <sheetPr/>
   <dimension ref="A1:Q1075"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="$A10:$XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A9" sqref="$A9:$XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5333333333333" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.0333333333333" customWidth="1"/>
     <col min="2" max="2" width="38.1" customWidth="1"/>
-    <col min="3" max="3" width="10.7833333333333" customWidth="1"/>
-    <col min="4" max="4" width="12.7166666666667" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
-    <col min="6" max="6" width="14.1416666666667" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7833333333333" customWidth="1"/>
-    <col min="8" max="8" width="26.3916666666667" customWidth="1"/>
+    <col min="3" max="3" width="10.7833333333333" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7166666666667" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1416666666667" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7833333333333" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26.3916666666667" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="11.2083333333333" customWidth="1"/>
     <col min="10" max="10" width="25.4" customWidth="1"/>
     <col min="11" max="12" width="11.75" customWidth="1"/>

</xml_diff>